<commit_message>
dan_chain_cfg_page update all component name according new name rule ok base
</commit_message>
<xml_diff>
--- a/pb01_gui_develop_record.xlsx
+++ b/pb01_gui_develop_record.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{B36CE81E-60B9-4316-AEE9-C562089A0BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC6433E3-0AD1-44F0-BF48-233A778017EC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C18C1A-A424-4187-93EF-B4F1119E1FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Index</t>
   </si>
@@ -126,6 +126,10 @@
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>控件命名规则：</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -209,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -217,13 +221,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -325,6 +332,50 @@
         <a:xfrm>
           <a:off x="7042114" y="647700"/>
           <a:ext cx="2231426" cy="1183134"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>11745</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60CE52D5-FECA-AA64-41F4-4EF04837E980}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4815840" y="1905000"/>
+          <a:ext cx="2270760" cy="964245"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -599,13 +650,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:T20"/>
+  <dimension ref="B2:T50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S4" sqref="S4:T10"/>
+      <selection pane="bottomRight" activeCell="N11" sqref="N11:R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,440 +665,1104 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4" t="s">
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="4"/>
+      <c r="T2" s="5"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
+      <c r="D11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
     </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="2"/>
+      <c r="T46" s="2"/>
+    </row>
+    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="2"/>
+      <c r="T48" s="2"/>
+    </row>
+    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+    </row>
+    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="50">
+    <mergeCell ref="B46:C50"/>
+    <mergeCell ref="D46:H50"/>
+    <mergeCell ref="I46:M50"/>
+    <mergeCell ref="N46:R50"/>
+    <mergeCell ref="S46:T50"/>
+    <mergeCell ref="B41:C45"/>
+    <mergeCell ref="D41:H45"/>
+    <mergeCell ref="I41:M45"/>
+    <mergeCell ref="N41:R45"/>
+    <mergeCell ref="S41:T45"/>
+    <mergeCell ref="B36:C40"/>
+    <mergeCell ref="D36:H40"/>
+    <mergeCell ref="I36:M40"/>
+    <mergeCell ref="N36:R40"/>
+    <mergeCell ref="S36:T40"/>
+    <mergeCell ref="B31:C35"/>
+    <mergeCell ref="D31:H35"/>
+    <mergeCell ref="I31:M35"/>
+    <mergeCell ref="N31:R35"/>
+    <mergeCell ref="S31:T35"/>
+    <mergeCell ref="B26:C30"/>
+    <mergeCell ref="D26:H30"/>
+    <mergeCell ref="I26:M30"/>
+    <mergeCell ref="N26:R30"/>
+    <mergeCell ref="S26:T30"/>
+    <mergeCell ref="B21:C25"/>
+    <mergeCell ref="D21:H25"/>
+    <mergeCell ref="I21:M25"/>
+    <mergeCell ref="N21:R25"/>
+    <mergeCell ref="S21:T25"/>
+    <mergeCell ref="B11:C15"/>
+    <mergeCell ref="D11:H15"/>
+    <mergeCell ref="I11:M15"/>
+    <mergeCell ref="N11:R15"/>
+    <mergeCell ref="S11:T15"/>
+    <mergeCell ref="B16:C20"/>
+    <mergeCell ref="D16:H20"/>
+    <mergeCell ref="I16:M20"/>
+    <mergeCell ref="N16:R20"/>
+    <mergeCell ref="S16:T20"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:H3"/>
+    <mergeCell ref="I2:M3"/>
+    <mergeCell ref="N2:R3"/>
+    <mergeCell ref="S2:T3"/>
     <mergeCell ref="B4:C10"/>
     <mergeCell ref="D4:H10"/>
     <mergeCell ref="I4:M10"/>
     <mergeCell ref="N4:R10"/>
     <mergeCell ref="S4:T10"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:H3"/>
-    <mergeCell ref="I2:M3"/>
-    <mergeCell ref="N2:R3"/>
-    <mergeCell ref="S2:T3"/>
-    <mergeCell ref="B16:C20"/>
-    <mergeCell ref="D16:H20"/>
-    <mergeCell ref="I16:M20"/>
-    <mergeCell ref="N16:R20"/>
-    <mergeCell ref="S16:T20"/>
-    <mergeCell ref="B11:C15"/>
-    <mergeCell ref="D11:H15"/>
-    <mergeCell ref="I11:M15"/>
-    <mergeCell ref="N11:R15"/>
-    <mergeCell ref="S11:T15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
set_table_head accept 0 for table height and pb01_gui_main add mea_acq_detail_data page table ok base
</commit_message>
<xml_diff>
--- a/pb01_gui_develop_record.xlsx
+++ b/pb01_gui_develop_record.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C18C1A-A424-4187-93EF-B4F1119E1FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFCB76B-E7D7-4E15-BAE3-6494AC8518E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Index</t>
   </si>
@@ -128,6 +128,187 @@
   </si>
   <si>
     <t>控件命名规则：</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">table </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">初始化的位置，除了在 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">initUI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">函数下外，在 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">slot_radio_single_dual_afe </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">函数也有，此函数包含 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">dev0 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">和 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">dev1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>切换时，要初始化的部分。</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NoneType' object has no attribute 'setBackground' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>报错的原因：</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">table </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">控件调用 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">setBackground </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">函数设置某个 item 的背景颜色时，要注意：调用此函数前，必须保证 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">table </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">对应的 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">item </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>已经被初始化，及要先在该 item 中填入一个值后再设置背景颜色。所以调用这个函数前，要先调用自己写的 set_table_item 函数，这里面有给各 item 值填入初始化值的操作，也可以不用此函数，直接给 item 填入值也可以。</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -213,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -231,6 +412,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -261,9 +445,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>274321</xdr:colOff>
+      <xdr:colOff>285751</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>164691</xdr:rowOff>
+      <xdr:rowOff>172311</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -343,15 +527,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>57151</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>11745</xdr:rowOff>
+      <xdr:colOff>472441</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -374,8 +558,140 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4815840" y="1905000"/>
-          <a:ext cx="2270760" cy="964245"/>
+          <a:off x="4857751" y="1933576"/>
+          <a:ext cx="2207895" cy="895350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>45722</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>17642</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457201</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>168415</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87DC83BE-83DF-C360-11C1-ACF0C64F58AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4846322" y="2875142"/>
+          <a:ext cx="1011554" cy="905153"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>94315</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>53341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>201607</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>179071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75BB7D98-2476-6BAF-743D-FD2ADDFB67DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1894540" y="4434841"/>
+          <a:ext cx="2507592" cy="506730"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>120015</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>89129</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>530396</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>170957</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="图片 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC279F75-C438-62C2-E2B1-0C3A7F337156}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7920990" y="3899129"/>
+          <a:ext cx="4010831" cy="1796328"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -650,13 +966,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:T50"/>
+  <dimension ref="B2:T56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N11" sqref="N11:R15"/>
+      <selection pane="bottomRight" activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,9 +1293,13 @@
       <c r="T15" s="2"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>3</v>
+      </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1082,14 +1402,20 @@
       <c r="T20" s="2"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <v>4</v>
+      </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="4"/>
+      <c r="D21" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="I21" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
@@ -1711,38 +2037,164 @@
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
     </row>
+    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="2"/>
+      <c r="T51" s="2"/>
+    </row>
+    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="2"/>
+      <c r="T52" s="2"/>
+    </row>
+    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
+      <c r="S53" s="2"/>
+      <c r="T53" s="2"/>
+    </row>
+    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="2"/>
+      <c r="T54" s="2"/>
+    </row>
+    <row r="55" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
+      <c r="S55" s="2"/>
+      <c r="T55" s="2"/>
+    </row>
+    <row r="56" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="B46:C50"/>
-    <mergeCell ref="D46:H50"/>
-    <mergeCell ref="I46:M50"/>
-    <mergeCell ref="N46:R50"/>
-    <mergeCell ref="S46:T50"/>
-    <mergeCell ref="B41:C45"/>
-    <mergeCell ref="D41:H45"/>
-    <mergeCell ref="I41:M45"/>
-    <mergeCell ref="N41:R45"/>
-    <mergeCell ref="S41:T45"/>
-    <mergeCell ref="B36:C40"/>
-    <mergeCell ref="D36:H40"/>
-    <mergeCell ref="I36:M40"/>
-    <mergeCell ref="N36:R40"/>
-    <mergeCell ref="S36:T40"/>
-    <mergeCell ref="B31:C35"/>
-    <mergeCell ref="D31:H35"/>
-    <mergeCell ref="I31:M35"/>
-    <mergeCell ref="N31:R35"/>
-    <mergeCell ref="S31:T35"/>
-    <mergeCell ref="B26:C30"/>
-    <mergeCell ref="D26:H30"/>
-    <mergeCell ref="I26:M30"/>
-    <mergeCell ref="N26:R30"/>
-    <mergeCell ref="S26:T30"/>
-    <mergeCell ref="B21:C25"/>
-    <mergeCell ref="D21:H25"/>
-    <mergeCell ref="I21:M25"/>
-    <mergeCell ref="N21:R25"/>
-    <mergeCell ref="S21:T25"/>
+    <mergeCell ref="B52:C56"/>
+    <mergeCell ref="D52:H56"/>
+    <mergeCell ref="I52:M56"/>
+    <mergeCell ref="N52:R56"/>
+    <mergeCell ref="S52:T56"/>
+    <mergeCell ref="B47:C51"/>
+    <mergeCell ref="D47:H51"/>
+    <mergeCell ref="I47:M51"/>
+    <mergeCell ref="N47:R51"/>
+    <mergeCell ref="S47:T51"/>
+    <mergeCell ref="B42:C46"/>
+    <mergeCell ref="D42:H46"/>
+    <mergeCell ref="I42:M46"/>
+    <mergeCell ref="N42:R46"/>
+    <mergeCell ref="S42:T46"/>
+    <mergeCell ref="B37:C41"/>
+    <mergeCell ref="D37:H41"/>
+    <mergeCell ref="I37:M41"/>
+    <mergeCell ref="N37:R41"/>
+    <mergeCell ref="S37:T41"/>
+    <mergeCell ref="B32:C36"/>
+    <mergeCell ref="D32:H36"/>
+    <mergeCell ref="I32:M36"/>
+    <mergeCell ref="N32:R36"/>
+    <mergeCell ref="S32:T36"/>
+    <mergeCell ref="B21:C31"/>
+    <mergeCell ref="D21:H31"/>
+    <mergeCell ref="I21:M31"/>
+    <mergeCell ref="N21:R31"/>
+    <mergeCell ref="S21:T31"/>
     <mergeCell ref="B11:C15"/>
     <mergeCell ref="D11:H15"/>
     <mergeCell ref="I11:M15"/>

</xml_diff>

<commit_message>
add init_tab_pages and complete chainCfgPage functions ok base
</commit_message>
<xml_diff>
--- a/pb01_gui_develop_record.xlsx
+++ b/pb01_gui_develop_record.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{0D325905-AFF9-4647-B230-73E94501D303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58F3E721-64EB-48D9-9195-693926E8D0C7}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{0D325905-AFF9-4647-B230-73E94501D303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C64FE35A-641B-461B-9917-CFDCF21D6542}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="develop" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Index</t>
   </si>
@@ -253,6 +253,203 @@
         <charset val="134"/>
       </rPr>
       <t>列表的 0 位置，对应着 status 寄存器变量的 bit15,所以用 0x8000 开始右移设置</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">在 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">initial daisy-chain </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">之前，一定要先初始化 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>bridge (max17841)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">初始化 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">max17841 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>在两个地方执行：</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. open_hid </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">中，连接 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">bridge </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>后马上初始化 17841</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. chainCfgPage </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">执行 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">POR </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>后</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">POR </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">执行后，一定要等一段时间才能再重新 初始化 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>daisy-chain</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，否则程序容易退出。</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -350,6 +547,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -358,9 +558,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -645,6 +842,226 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>28342</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>119696</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>182770</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D523841-2845-3C5E-93EA-366A7DD6FEB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4899660" y="5933842"/>
+          <a:ext cx="10871516" cy="535428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>215735</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>243841</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>29142</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="图片 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCE6DFE6-AEB1-6DC3-3D6C-AB69E067E5A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2021675" y="6553200"/>
+          <a:ext cx="1834046" cy="905442"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>86188</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>30479</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>146587</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="图片 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC103362-DDC0-73EF-7B8C-91B7D0034F78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4902028" y="8039100"/>
+          <a:ext cx="2352211" cy="1060987"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>60301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>99061</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>130144</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="图片 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE6CBC0D-CB2F-285B-5A64-52E1C01046C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7901941" y="7870801"/>
+          <a:ext cx="3634740" cy="1212843"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>53197</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>159769</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="图片 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09869F86-E4AA-3EE2-5816-071175056976}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4869037" y="9182100"/>
+          <a:ext cx="1455564" cy="883669"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -695,6 +1112,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -960,13 +1381,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:T56"/>
+  <dimension ref="B2:T63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N37" sqref="N37:R41"/>
+      <selection pane="bottomRight" activeCell="I49" sqref="I49:M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,63 +1396,63 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6" t="s">
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6" t="s">
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="6"/>
+      <c r="T2" s="7"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="3"/>
@@ -1182,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="3"/>
@@ -1400,7 +1821,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="3"/>
@@ -1826,19 +2247,27 @@
       <c r="T40" s="2"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B41" s="2"/>
+      <c r="B41" s="2">
+        <v>6</v>
+      </c>
       <c r="C41" s="2"/>
-      <c r="D41" s="3"/>
+      <c r="D41" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
+      <c r="I41" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
+      <c r="N41" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
@@ -1994,9 +2423,13 @@
       <c r="T48" s="2"/>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="2"/>
+      <c r="B49" s="2">
+        <v>7</v>
+      </c>
       <c r="C49" s="2"/>
-      <c r="D49" s="3"/>
+      <c r="D49" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -2160,6 +2593,153 @@
       <c r="R56" s="3"/>
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
+    </row>
+    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="2"/>
+      <c r="T57" s="2"/>
+    </row>
+    <row r="58" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="2"/>
+      <c r="T58" s="2"/>
+    </row>
+    <row r="59" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="2"/>
+      <c r="T59" s="2"/>
+    </row>
+    <row r="60" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="2"/>
+      <c r="T60" s="2"/>
+    </row>
+    <row r="61" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="3"/>
+      <c r="O61" s="3"/>
+      <c r="P61" s="3"/>
+      <c r="Q61" s="3"/>
+      <c r="R61" s="3"/>
+      <c r="S61" s="2"/>
+      <c r="T61" s="2"/>
+    </row>
+    <row r="62" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="2"/>
+      <c r="T62" s="2"/>
+    </row>
+    <row r="63" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="2"/>
+      <c r="T63" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="50">
@@ -2188,31 +2768,31 @@
     <mergeCell ref="I21:M31"/>
     <mergeCell ref="N21:R31"/>
     <mergeCell ref="S21:T31"/>
-    <mergeCell ref="B32:C36"/>
-    <mergeCell ref="D32:H36"/>
-    <mergeCell ref="I32:M36"/>
-    <mergeCell ref="N32:R36"/>
-    <mergeCell ref="S32:T36"/>
-    <mergeCell ref="B37:C41"/>
-    <mergeCell ref="D37:H41"/>
-    <mergeCell ref="I37:M41"/>
-    <mergeCell ref="N37:R41"/>
-    <mergeCell ref="S37:T41"/>
-    <mergeCell ref="B42:C46"/>
-    <mergeCell ref="D42:H46"/>
-    <mergeCell ref="I42:M46"/>
-    <mergeCell ref="N42:R46"/>
-    <mergeCell ref="S42:T46"/>
-    <mergeCell ref="B47:C51"/>
-    <mergeCell ref="D47:H51"/>
-    <mergeCell ref="I47:M51"/>
-    <mergeCell ref="N47:R51"/>
-    <mergeCell ref="S47:T51"/>
-    <mergeCell ref="B52:C56"/>
-    <mergeCell ref="D52:H56"/>
-    <mergeCell ref="I52:M56"/>
-    <mergeCell ref="N52:R56"/>
-    <mergeCell ref="S52:T56"/>
+    <mergeCell ref="B32:C40"/>
+    <mergeCell ref="D32:H40"/>
+    <mergeCell ref="I32:M40"/>
+    <mergeCell ref="N32:R40"/>
+    <mergeCell ref="S32:T40"/>
+    <mergeCell ref="B41:C48"/>
+    <mergeCell ref="D41:H48"/>
+    <mergeCell ref="I41:M48"/>
+    <mergeCell ref="N41:R48"/>
+    <mergeCell ref="S41:T48"/>
+    <mergeCell ref="B49:C53"/>
+    <mergeCell ref="D49:H53"/>
+    <mergeCell ref="I49:M53"/>
+    <mergeCell ref="N49:R53"/>
+    <mergeCell ref="S49:T53"/>
+    <mergeCell ref="B54:C58"/>
+    <mergeCell ref="D54:H58"/>
+    <mergeCell ref="I54:M58"/>
+    <mergeCell ref="N54:R58"/>
+    <mergeCell ref="S54:T58"/>
+    <mergeCell ref="B59:C63"/>
+    <mergeCell ref="D59:H63"/>
+    <mergeCell ref="I59:M63"/>
+    <mergeCell ref="N59:R63"/>
+    <mergeCell ref="S59:T63"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2235,63 +2815,63 @@
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6" t="s">
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6" t="s">
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="6"/>
+      <c r="T2" s="7"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="3"/>
@@ -2400,7 +2980,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -2612,7 +3192,7 @@
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="7"/>
+      <c r="D19" s="4"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -2717,7 +3297,7 @@
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="5"/>
+      <c r="D24" s="6"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>

</xml_diff>

<commit_message>
add pb01_17841_alert_packet and run ok base
</commit_message>
<xml_diff>
--- a/pb01_gui_develop_record.xlsx
+++ b/pb01_gui_develop_record.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{0D325905-AFF9-4647-B230-73E94501D303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39D21B8C-1F25-4F9C-8B53-27BDDF18A01D}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{0D325905-AFF9-4647-B230-73E94501D303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D89B9BC5-6188-483B-B456-8585B1818C05}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="develop" sheetId="1" r:id="rId1"/>
@@ -1291,20 +1291,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1985,6 +1985,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>483335</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="图片 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BB99234-9289-90B4-1579-EEDF0F45314F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4884420" y="12534900"/>
+          <a:ext cx="2822675" cy="579120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2310,7 +2354,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I59" sqref="I59:M73"/>
+      <selection pane="bottomRight" activeCell="S59" sqref="S59:T73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2319,163 +2363,163 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7" t="s">
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7" t="s">
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="7"/>
+      <c r="T2" s="4"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
@@ -2484,149 +2528,149 @@
         <v>2</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
     </row>
@@ -2635,107 +2679,107 @@
         <v>3</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
     </row>
@@ -2744,107 +2788,107 @@
         <v>4</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
     </row>
@@ -2856,232 +2900,232 @@
       <c r="D26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4" t="s">
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
       <c r="S35" s="2"/>
       <c r="T35" s="2"/>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
       <c r="S36" s="2"/>
       <c r="T36" s="2"/>
     </row>
@@ -3090,191 +3134,191 @@
         <v>6</v>
       </c>
       <c r="C37" s="2"/>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
       <c r="S39" s="2"/>
       <c r="T39" s="2"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-      <c r="P40" s="4"/>
-      <c r="Q40" s="4"/>
-      <c r="R40" s="4"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-      <c r="P41" s="4"/>
-      <c r="Q41" s="4"/>
-      <c r="R41" s="4"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
-      <c r="P42" s="4"/>
-      <c r="Q42" s="4"/>
-      <c r="R42" s="4"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
-      <c r="Q43" s="4"/>
-      <c r="R43" s="4"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
-      <c r="Q45" s="4"/>
-      <c r="R45" s="4"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
     </row>
@@ -3283,174 +3327,174 @@
         <v>7</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4" t="s">
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4" t="s">
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4"/>
-      <c r="Q46" s="4"/>
-      <c r="R46" s="4"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4"/>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="3"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
       <c r="S48" s="2"/>
       <c r="T48" s="2"/>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
-      <c r="P50" s="4"/>
-      <c r="Q50" s="4"/>
-      <c r="R50" s="4"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
-      <c r="P51" s="4"/>
-      <c r="Q51" s="4"/>
-      <c r="R51" s="4"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
     </row>
     <row r="52" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
-      <c r="N52" s="4"/>
-      <c r="O52" s="4"/>
-      <c r="P52" s="4"/>
-      <c r="Q52" s="4"/>
-      <c r="R52" s="4"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
-      <c r="P53" s="4"/>
-      <c r="Q53" s="4"/>
-      <c r="R53" s="4"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
     </row>
@@ -3459,107 +3503,107 @@
         <v>8</v>
       </c>
       <c r="C54" s="2"/>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
-      <c r="P54" s="4"/>
-      <c r="Q54" s="4"/>
-      <c r="R54" s="4"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="3"/>
+      <c r="R54" s="3"/>
       <c r="S54" s="2"/>
       <c r="T54" s="2"/>
     </row>
     <row r="55" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-      <c r="P55" s="4"/>
-      <c r="Q55" s="4"/>
-      <c r="R55" s="4"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="O55" s="3"/>
+      <c r="P55" s="3"/>
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
       <c r="S55" s="2"/>
       <c r="T55" s="2"/>
     </row>
     <row r="56" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
-      <c r="N56" s="4"/>
-      <c r="O56" s="4"/>
-      <c r="P56" s="4"/>
-      <c r="Q56" s="4"/>
-      <c r="R56" s="4"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
     </row>
     <row r="57" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
-      <c r="N57" s="4"/>
-      <c r="O57" s="4"/>
-      <c r="P57" s="4"/>
-      <c r="Q57" s="4"/>
-      <c r="R57" s="4"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
       <c r="S57" s="2"/>
       <c r="T57" s="2"/>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-      <c r="N58" s="4"/>
-      <c r="O58" s="4"/>
-      <c r="P58" s="4"/>
-      <c r="Q58" s="4"/>
-      <c r="R58" s="4"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
       <c r="S58" s="2"/>
       <c r="T58" s="2"/>
     </row>
@@ -3568,704 +3612,704 @@
         <v>9</v>
       </c>
       <c r="C59" s="2"/>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4" t="s">
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
-      <c r="P59" s="4"/>
-      <c r="Q59" s="4"/>
-      <c r="R59" s="4"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
       <c r="S59" s="2"/>
       <c r="T59" s="2"/>
     </row>
     <row r="60" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
-      <c r="O60" s="4"/>
-      <c r="P60" s="4"/>
-      <c r="Q60" s="4"/>
-      <c r="R60" s="4"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
       <c r="S60" s="2"/>
       <c r="T60" s="2"/>
     </row>
     <row r="61" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
-      <c r="P61" s="4"/>
-      <c r="Q61" s="4"/>
-      <c r="R61" s="4"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="3"/>
+      <c r="O61" s="3"/>
+      <c r="P61" s="3"/>
+      <c r="Q61" s="3"/>
+      <c r="R61" s="3"/>
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
     </row>
     <row r="62" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
-      <c r="M62" s="4"/>
-      <c r="N62" s="4"/>
-      <c r="O62" s="4"/>
-      <c r="P62" s="4"/>
-      <c r="Q62" s="4"/>
-      <c r="R62" s="4"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
     </row>
     <row r="63" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
-      <c r="P63" s="4"/>
-      <c r="Q63" s="4"/>
-      <c r="R63" s="4"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
       <c r="S63" s="2"/>
       <c r="T63" s="2"/>
     </row>
     <row r="64" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-      <c r="M64" s="4"/>
-      <c r="N64" s="4"/>
-      <c r="O64" s="4"/>
-      <c r="P64" s="4"/>
-      <c r="Q64" s="4"/>
-      <c r="R64" s="4"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
+      <c r="M64" s="3"/>
+      <c r="N64" s="3"/>
+      <c r="O64" s="3"/>
+      <c r="P64" s="3"/>
+      <c r="Q64" s="3"/>
+      <c r="R64" s="3"/>
       <c r="S64" s="2"/>
       <c r="T64" s="2"/>
     </row>
     <row r="65" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
-      <c r="M65" s="4"/>
-      <c r="N65" s="4"/>
-      <c r="O65" s="4"/>
-      <c r="P65" s="4"/>
-      <c r="Q65" s="4"/>
-      <c r="R65" s="4"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+      <c r="P65" s="3"/>
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
       <c r="S65" s="2"/>
       <c r="T65" s="2"/>
     </row>
     <row r="66" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
-      <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
-      <c r="P66" s="4"/>
-      <c r="Q66" s="4"/>
-      <c r="R66" s="4"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+      <c r="P66" s="3"/>
+      <c r="Q66" s="3"/>
+      <c r="R66" s="3"/>
       <c r="S66" s="2"/>
       <c r="T66" s="2"/>
     </row>
     <row r="67" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
-      <c r="M67" s="4"/>
-      <c r="N67" s="4"/>
-      <c r="O67" s="4"/>
-      <c r="P67" s="4"/>
-      <c r="Q67" s="4"/>
-      <c r="R67" s="4"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
       <c r="S67" s="2"/>
       <c r="T67" s="2"/>
     </row>
     <row r="68" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-      <c r="I68" s="4"/>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
-      <c r="M68" s="4"/>
-      <c r="N68" s="4"/>
-      <c r="O68" s="4"/>
-      <c r="P68" s="4"/>
-      <c r="Q68" s="4"/>
-      <c r="R68" s="4"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
       <c r="S68" s="2"/>
       <c r="T68" s="2"/>
     </row>
     <row r="69" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
-      <c r="I69" s="4"/>
-      <c r="J69" s="4"/>
-      <c r="K69" s="4"/>
-      <c r="L69" s="4"/>
-      <c r="M69" s="4"/>
-      <c r="N69" s="4"/>
-      <c r="O69" s="4"/>
-      <c r="P69" s="4"/>
-      <c r="Q69" s="4"/>
-      <c r="R69" s="4"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="3"/>
+      <c r="N69" s="3"/>
+      <c r="O69" s="3"/>
+      <c r="P69" s="3"/>
+      <c r="Q69" s="3"/>
+      <c r="R69" s="3"/>
       <c r="S69" s="2"/>
       <c r="T69" s="2"/>
     </row>
     <row r="70" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
-      <c r="J70" s="4"/>
-      <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
-      <c r="M70" s="4"/>
-      <c r="N70" s="4"/>
-      <c r="O70" s="4"/>
-      <c r="P70" s="4"/>
-      <c r="Q70" s="4"/>
-      <c r="R70" s="4"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="3"/>
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
       <c r="S70" s="2"/>
       <c r="T70" s="2"/>
     </row>
     <row r="71" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
-      <c r="N71" s="4"/>
-      <c r="O71" s="4"/>
-      <c r="P71" s="4"/>
-      <c r="Q71" s="4"/>
-      <c r="R71" s="4"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="3"/>
+      <c r="O71" s="3"/>
+      <c r="P71" s="3"/>
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
       <c r="S71" s="2"/>
       <c r="T71" s="2"/>
     </row>
     <row r="72" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="4"/>
-      <c r="J72" s="4"/>
-      <c r="K72" s="4"/>
-      <c r="L72" s="4"/>
-      <c r="M72" s="4"/>
-      <c r="N72" s="4"/>
-      <c r="O72" s="4"/>
-      <c r="P72" s="4"/>
-      <c r="Q72" s="4"/>
-      <c r="R72" s="4"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
+      <c r="M72" s="3"/>
+      <c r="N72" s="3"/>
+      <c r="O72" s="3"/>
+      <c r="P72" s="3"/>
+      <c r="Q72" s="3"/>
+      <c r="R72" s="3"/>
       <c r="S72" s="2"/>
       <c r="T72" s="2"/>
     </row>
     <row r="73" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
-      <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="4"/>
-      <c r="K73" s="4"/>
-      <c r="L73" s="4"/>
-      <c r="M73" s="4"/>
-      <c r="N73" s="4"/>
-      <c r="O73" s="4"/>
-      <c r="P73" s="4"/>
-      <c r="Q73" s="4"/>
-      <c r="R73" s="4"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3"/>
+      <c r="N73" s="3"/>
+      <c r="O73" s="3"/>
+      <c r="P73" s="3"/>
+      <c r="Q73" s="3"/>
+      <c r="R73" s="3"/>
       <c r="S73" s="2"/>
       <c r="T73" s="2"/>
     </row>
     <row r="74" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="4"/>
-      <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
-      <c r="I74" s="4"/>
-      <c r="J74" s="4"/>
-      <c r="K74" s="4"/>
-      <c r="L74" s="4"/>
-      <c r="M74" s="4"/>
-      <c r="N74" s="4"/>
-      <c r="O74" s="4"/>
-      <c r="P74" s="4"/>
-      <c r="Q74" s="4"/>
-      <c r="R74" s="4"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+      <c r="M74" s="3"/>
+      <c r="N74" s="3"/>
+      <c r="O74" s="3"/>
+      <c r="P74" s="3"/>
+      <c r="Q74" s="3"/>
+      <c r="R74" s="3"/>
       <c r="S74" s="2"/>
       <c r="T74" s="2"/>
     </row>
     <row r="75" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
-      <c r="I75" s="4"/>
-      <c r="J75" s="4"/>
-      <c r="K75" s="4"/>
-      <c r="L75" s="4"/>
-      <c r="M75" s="4"/>
-      <c r="N75" s="4"/>
-      <c r="O75" s="4"/>
-      <c r="P75" s="4"/>
-      <c r="Q75" s="4"/>
-      <c r="R75" s="4"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="3"/>
+      <c r="P75" s="3"/>
+      <c r="Q75" s="3"/>
+      <c r="R75" s="3"/>
       <c r="S75" s="2"/>
       <c r="T75" s="2"/>
     </row>
     <row r="76" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="4"/>
-      <c r="G76" s="4"/>
-      <c r="H76" s="4"/>
-      <c r="I76" s="4"/>
-      <c r="J76" s="4"/>
-      <c r="K76" s="4"/>
-      <c r="L76" s="4"/>
-      <c r="M76" s="4"/>
-      <c r="N76" s="4"/>
-      <c r="O76" s="4"/>
-      <c r="P76" s="4"/>
-      <c r="Q76" s="4"/>
-      <c r="R76" s="4"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3"/>
+      <c r="N76" s="3"/>
+      <c r="O76" s="3"/>
+      <c r="P76" s="3"/>
+      <c r="Q76" s="3"/>
+      <c r="R76" s="3"/>
       <c r="S76" s="2"/>
       <c r="T76" s="2"/>
     </row>
     <row r="77" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4"/>
-      <c r="F77" s="4"/>
-      <c r="G77" s="4"/>
-      <c r="H77" s="4"/>
-      <c r="I77" s="4"/>
-      <c r="J77" s="4"/>
-      <c r="K77" s="4"/>
-      <c r="L77" s="4"/>
-      <c r="M77" s="4"/>
-      <c r="N77" s="4"/>
-      <c r="O77" s="4"/>
-      <c r="P77" s="4"/>
-      <c r="Q77" s="4"/>
-      <c r="R77" s="4"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+      <c r="N77" s="3"/>
+      <c r="O77" s="3"/>
+      <c r="P77" s="3"/>
+      <c r="Q77" s="3"/>
+      <c r="R77" s="3"/>
       <c r="S77" s="2"/>
       <c r="T77" s="2"/>
     </row>
     <row r="78" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
-      <c r="G78" s="4"/>
-      <c r="H78" s="4"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="4"/>
-      <c r="K78" s="4"/>
-      <c r="L78" s="4"/>
-      <c r="M78" s="4"/>
-      <c r="N78" s="4"/>
-      <c r="O78" s="4"/>
-      <c r="P78" s="4"/>
-      <c r="Q78" s="4"/>
-      <c r="R78" s="4"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="3"/>
+      <c r="P78" s="3"/>
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3"/>
       <c r="S78" s="2"/>
       <c r="T78" s="2"/>
     </row>
     <row r="79" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
-      <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
-      <c r="I79" s="4"/>
-      <c r="J79" s="4"/>
-      <c r="K79" s="4"/>
-      <c r="L79" s="4"/>
-      <c r="M79" s="4"/>
-      <c r="N79" s="4"/>
-      <c r="O79" s="4"/>
-      <c r="P79" s="4"/>
-      <c r="Q79" s="4"/>
-      <c r="R79" s="4"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+      <c r="M79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="O79" s="3"/>
+      <c r="P79" s="3"/>
+      <c r="Q79" s="3"/>
+      <c r="R79" s="3"/>
       <c r="S79" s="2"/>
       <c r="T79" s="2"/>
     </row>
     <row r="80" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
-      <c r="G80" s="4"/>
-      <c r="H80" s="4"/>
-      <c r="I80" s="4"/>
-      <c r="J80" s="4"/>
-      <c r="K80" s="4"/>
-      <c r="L80" s="4"/>
-      <c r="M80" s="4"/>
-      <c r="N80" s="4"/>
-      <c r="O80" s="4"/>
-      <c r="P80" s="4"/>
-      <c r="Q80" s="4"/>
-      <c r="R80" s="4"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="M80" s="3"/>
+      <c r="N80" s="3"/>
+      <c r="O80" s="3"/>
+      <c r="P80" s="3"/>
+      <c r="Q80" s="3"/>
+      <c r="R80" s="3"/>
       <c r="S80" s="2"/>
       <c r="T80" s="2"/>
     </row>
     <row r="81" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
-      <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
-      <c r="I81" s="4"/>
-      <c r="J81" s="4"/>
-      <c r="K81" s="4"/>
-      <c r="L81" s="4"/>
-      <c r="M81" s="4"/>
-      <c r="N81" s="4"/>
-      <c r="O81" s="4"/>
-      <c r="P81" s="4"/>
-      <c r="Q81" s="4"/>
-      <c r="R81" s="4"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
+      <c r="K81" s="3"/>
+      <c r="L81" s="3"/>
+      <c r="M81" s="3"/>
+      <c r="N81" s="3"/>
+      <c r="O81" s="3"/>
+      <c r="P81" s="3"/>
+      <c r="Q81" s="3"/>
+      <c r="R81" s="3"/>
       <c r="S81" s="2"/>
       <c r="T81" s="2"/>
     </row>
     <row r="82" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
-      <c r="H82" s="4"/>
-      <c r="I82" s="4"/>
-      <c r="J82" s="4"/>
-      <c r="K82" s="4"/>
-      <c r="L82" s="4"/>
-      <c r="M82" s="4"/>
-      <c r="N82" s="4"/>
-      <c r="O82" s="4"/>
-      <c r="P82" s="4"/>
-      <c r="Q82" s="4"/>
-      <c r="R82" s="4"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
+      <c r="M82" s="3"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="3"/>
+      <c r="P82" s="3"/>
+      <c r="Q82" s="3"/>
+      <c r="R82" s="3"/>
       <c r="S82" s="2"/>
       <c r="T82" s="2"/>
     </row>
     <row r="83" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
-      <c r="D83" s="4"/>
-      <c r="E83" s="4"/>
-      <c r="F83" s="4"/>
-      <c r="G83" s="4"/>
-      <c r="H83" s="4"/>
-      <c r="I83" s="4"/>
-      <c r="J83" s="4"/>
-      <c r="K83" s="4"/>
-      <c r="L83" s="4"/>
-      <c r="M83" s="4"/>
-      <c r="N83" s="4"/>
-      <c r="O83" s="4"/>
-      <c r="P83" s="4"/>
-      <c r="Q83" s="4"/>
-      <c r="R83" s="4"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
+      <c r="M83" s="3"/>
+      <c r="N83" s="3"/>
+      <c r="O83" s="3"/>
+      <c r="P83" s="3"/>
+      <c r="Q83" s="3"/>
+      <c r="R83" s="3"/>
       <c r="S83" s="2"/>
       <c r="T83" s="2"/>
     </row>
     <row r="84" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4"/>
-      <c r="G84" s="4"/>
-      <c r="H84" s="4"/>
-      <c r="I84" s="4"/>
-      <c r="J84" s="4"/>
-      <c r="K84" s="4"/>
-      <c r="L84" s="4"/>
-      <c r="M84" s="4"/>
-      <c r="N84" s="4"/>
-      <c r="O84" s="4"/>
-      <c r="P84" s="4"/>
-      <c r="Q84" s="4"/>
-      <c r="R84" s="4"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="3"/>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+      <c r="L84" s="3"/>
+      <c r="M84" s="3"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="3"/>
+      <c r="P84" s="3"/>
+      <c r="Q84" s="3"/>
+      <c r="R84" s="3"/>
       <c r="S84" s="2"/>
       <c r="T84" s="2"/>
     </row>
     <row r="85" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
-      <c r="G85" s="4"/>
-      <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
-      <c r="J85" s="4"/>
-      <c r="K85" s="4"/>
-      <c r="L85" s="4"/>
-      <c r="M85" s="4"/>
-      <c r="N85" s="4"/>
-      <c r="O85" s="4"/>
-      <c r="P85" s="4"/>
-      <c r="Q85" s="4"/>
-      <c r="R85" s="4"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="3"/>
+      <c r="L85" s="3"/>
+      <c r="M85" s="3"/>
+      <c r="N85" s="3"/>
+      <c r="O85" s="3"/>
+      <c r="P85" s="3"/>
+      <c r="Q85" s="3"/>
+      <c r="R85" s="3"/>
       <c r="S85" s="2"/>
       <c r="T85" s="2"/>
     </row>
     <row r="86" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
-      <c r="H86" s="4"/>
-      <c r="I86" s="4"/>
-      <c r="J86" s="4"/>
-      <c r="K86" s="4"/>
-      <c r="L86" s="4"/>
-      <c r="M86" s="4"/>
-      <c r="N86" s="4"/>
-      <c r="O86" s="4"/>
-      <c r="P86" s="4"/>
-      <c r="Q86" s="4"/>
-      <c r="R86" s="4"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="3"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="3"/>
+      <c r="P86" s="3"/>
+      <c r="Q86" s="3"/>
+      <c r="R86" s="3"/>
       <c r="S86" s="2"/>
       <c r="T86" s="2"/>
     </row>
     <row r="87" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="4"/>
-      <c r="G87" s="4"/>
-      <c r="H87" s="4"/>
-      <c r="I87" s="4"/>
-      <c r="J87" s="4"/>
-      <c r="K87" s="4"/>
-      <c r="L87" s="4"/>
-      <c r="M87" s="4"/>
-      <c r="N87" s="4"/>
-      <c r="O87" s="4"/>
-      <c r="P87" s="4"/>
-      <c r="Q87" s="4"/>
-      <c r="R87" s="4"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="I87" s="3"/>
+      <c r="J87" s="3"/>
+      <c r="K87" s="3"/>
+      <c r="L87" s="3"/>
+      <c r="M87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="O87" s="3"/>
+      <c r="P87" s="3"/>
+      <c r="Q87" s="3"/>
+      <c r="R87" s="3"/>
       <c r="S87" s="2"/>
       <c r="T87" s="2"/>
     </row>
     <row r="88" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
-      <c r="H88" s="4"/>
-      <c r="I88" s="4"/>
-      <c r="J88" s="4"/>
-      <c r="K88" s="4"/>
-      <c r="L88" s="4"/>
-      <c r="M88" s="4"/>
-      <c r="N88" s="4"/>
-      <c r="O88" s="4"/>
-      <c r="P88" s="4"/>
-      <c r="Q88" s="4"/>
-      <c r="R88" s="4"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="3"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="3"/>
+      <c r="P88" s="3"/>
+      <c r="Q88" s="3"/>
+      <c r="R88" s="3"/>
       <c r="S88" s="2"/>
       <c r="T88" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="B4:C8"/>
+    <mergeCell ref="D4:H8"/>
+    <mergeCell ref="I4:M8"/>
+    <mergeCell ref="N4:R8"/>
+    <mergeCell ref="S4:T8"/>
+    <mergeCell ref="B74:C78"/>
+    <mergeCell ref="D74:H78"/>
+    <mergeCell ref="I74:M78"/>
+    <mergeCell ref="N74:R78"/>
+    <mergeCell ref="S74:T78"/>
+    <mergeCell ref="B59:C73"/>
+    <mergeCell ref="D59:H73"/>
+    <mergeCell ref="I59:M73"/>
+    <mergeCell ref="N59:R73"/>
+    <mergeCell ref="S59:T73"/>
+    <mergeCell ref="B54:C58"/>
+    <mergeCell ref="D54:H58"/>
+    <mergeCell ref="I54:M58"/>
+    <mergeCell ref="N54:R58"/>
+    <mergeCell ref="S54:T58"/>
+    <mergeCell ref="B46:C53"/>
+    <mergeCell ref="D46:H53"/>
+    <mergeCell ref="I46:M53"/>
+    <mergeCell ref="N46:R53"/>
+    <mergeCell ref="S46:T53"/>
+    <mergeCell ref="B37:C45"/>
+    <mergeCell ref="D37:H45"/>
+    <mergeCell ref="I37:M45"/>
+    <mergeCell ref="N37:R45"/>
+    <mergeCell ref="S37:T45"/>
+    <mergeCell ref="B26:C36"/>
+    <mergeCell ref="D26:H36"/>
+    <mergeCell ref="I26:M36"/>
+    <mergeCell ref="N26:R36"/>
+    <mergeCell ref="S26:T36"/>
+    <mergeCell ref="B16:C20"/>
+    <mergeCell ref="D16:H20"/>
+    <mergeCell ref="I16:M20"/>
+    <mergeCell ref="N16:R20"/>
+    <mergeCell ref="S16:T20"/>
+    <mergeCell ref="B21:C25"/>
+    <mergeCell ref="D21:H25"/>
+    <mergeCell ref="I21:M25"/>
+    <mergeCell ref="N21:R25"/>
+    <mergeCell ref="S21:T25"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:H3"/>
+    <mergeCell ref="I2:M3"/>
+    <mergeCell ref="N2:R3"/>
+    <mergeCell ref="S2:T3"/>
+    <mergeCell ref="B9:C15"/>
+    <mergeCell ref="D9:H15"/>
+    <mergeCell ref="I9:M15"/>
+    <mergeCell ref="N9:R15"/>
+    <mergeCell ref="S9:T15"/>
+    <mergeCell ref="B79:C83"/>
+    <mergeCell ref="D79:H83"/>
+    <mergeCell ref="I79:M83"/>
+    <mergeCell ref="N79:R83"/>
+    <mergeCell ref="S79:T83"/>
     <mergeCell ref="B84:C88"/>
     <mergeCell ref="D84:H88"/>
     <mergeCell ref="I84:M88"/>
     <mergeCell ref="N84:R88"/>
     <mergeCell ref="S84:T88"/>
-    <mergeCell ref="B79:C83"/>
-    <mergeCell ref="D79:H83"/>
-    <mergeCell ref="I79:M83"/>
-    <mergeCell ref="N79:R83"/>
-    <mergeCell ref="S79:T83"/>
-    <mergeCell ref="B9:C15"/>
-    <mergeCell ref="D9:H15"/>
-    <mergeCell ref="I9:M15"/>
-    <mergeCell ref="N9:R15"/>
-    <mergeCell ref="S9:T15"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:H3"/>
-    <mergeCell ref="I2:M3"/>
-    <mergeCell ref="N2:R3"/>
-    <mergeCell ref="S2:T3"/>
-    <mergeCell ref="B21:C25"/>
-    <mergeCell ref="D21:H25"/>
-    <mergeCell ref="I21:M25"/>
-    <mergeCell ref="N21:R25"/>
-    <mergeCell ref="S21:T25"/>
-    <mergeCell ref="B16:C20"/>
-    <mergeCell ref="D16:H20"/>
-    <mergeCell ref="I16:M20"/>
-    <mergeCell ref="N16:R20"/>
-    <mergeCell ref="S16:T20"/>
-    <mergeCell ref="B26:C36"/>
-    <mergeCell ref="D26:H36"/>
-    <mergeCell ref="I26:M36"/>
-    <mergeCell ref="N26:R36"/>
-    <mergeCell ref="S26:T36"/>
-    <mergeCell ref="B37:C45"/>
-    <mergeCell ref="D37:H45"/>
-    <mergeCell ref="I37:M45"/>
-    <mergeCell ref="N37:R45"/>
-    <mergeCell ref="S37:T45"/>
-    <mergeCell ref="B46:C53"/>
-    <mergeCell ref="D46:H53"/>
-    <mergeCell ref="I46:M53"/>
-    <mergeCell ref="N46:R53"/>
-    <mergeCell ref="S46:T53"/>
-    <mergeCell ref="B54:C58"/>
-    <mergeCell ref="D54:H58"/>
-    <mergeCell ref="I54:M58"/>
-    <mergeCell ref="N54:R58"/>
-    <mergeCell ref="S54:T58"/>
-    <mergeCell ref="B59:C73"/>
-    <mergeCell ref="D59:H73"/>
-    <mergeCell ref="I59:M73"/>
-    <mergeCell ref="N59:R73"/>
-    <mergeCell ref="S59:T73"/>
-    <mergeCell ref="B74:C78"/>
-    <mergeCell ref="D74:H78"/>
-    <mergeCell ref="I74:M78"/>
-    <mergeCell ref="N74:R78"/>
-    <mergeCell ref="S74:T78"/>
-    <mergeCell ref="B4:C8"/>
-    <mergeCell ref="D4:H8"/>
-    <mergeCell ref="I4:M8"/>
-    <mergeCell ref="N4:R8"/>
-    <mergeCell ref="S4:T8"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4288,163 +4332,163 @@
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7" t="s">
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7" t="s">
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="7"/>
+      <c r="T2" s="4"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
@@ -4453,105 +4497,105 @@
         <v>2</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
     </row>
@@ -4560,460 +4604,460 @@
         <v>3</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B29:C33"/>
+    <mergeCell ref="D29:H33"/>
+    <mergeCell ref="I29:M33"/>
+    <mergeCell ref="N29:R33"/>
+    <mergeCell ref="S29:T33"/>
+    <mergeCell ref="B19:C23"/>
+    <mergeCell ref="D19:H23"/>
+    <mergeCell ref="I19:M23"/>
+    <mergeCell ref="N19:R23"/>
+    <mergeCell ref="S19:T23"/>
+    <mergeCell ref="B24:C28"/>
+    <mergeCell ref="D24:H28"/>
+    <mergeCell ref="I24:M28"/>
+    <mergeCell ref="N24:R28"/>
+    <mergeCell ref="S24:T28"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="D9:H13"/>
+    <mergeCell ref="I9:M13"/>
+    <mergeCell ref="N9:R13"/>
+    <mergeCell ref="S9:T13"/>
+    <mergeCell ref="B14:C18"/>
+    <mergeCell ref="D14:H18"/>
+    <mergeCell ref="I14:M18"/>
+    <mergeCell ref="N14:R18"/>
+    <mergeCell ref="S14:T18"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:H3"/>
+    <mergeCell ref="I2:M3"/>
+    <mergeCell ref="N2:R3"/>
+    <mergeCell ref="S2:T3"/>
     <mergeCell ref="B4:C8"/>
     <mergeCell ref="D4:H8"/>
     <mergeCell ref="I4:M8"/>
     <mergeCell ref="N4:R8"/>
     <mergeCell ref="S4:T8"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:H3"/>
-    <mergeCell ref="I2:M3"/>
-    <mergeCell ref="N2:R3"/>
-    <mergeCell ref="S2:T3"/>
-    <mergeCell ref="B14:C18"/>
-    <mergeCell ref="D14:H18"/>
-    <mergeCell ref="I14:M18"/>
-    <mergeCell ref="N14:R18"/>
-    <mergeCell ref="S14:T18"/>
-    <mergeCell ref="B9:C13"/>
-    <mergeCell ref="D9:H13"/>
-    <mergeCell ref="I9:M13"/>
-    <mergeCell ref="N9:R13"/>
-    <mergeCell ref="S9:T13"/>
-    <mergeCell ref="B24:C28"/>
-    <mergeCell ref="D24:H28"/>
-    <mergeCell ref="I24:M28"/>
-    <mergeCell ref="N24:R28"/>
-    <mergeCell ref="S24:T28"/>
-    <mergeCell ref="B19:C23"/>
-    <mergeCell ref="D19:H23"/>
-    <mergeCell ref="I19:M23"/>
-    <mergeCell ref="N19:R23"/>
-    <mergeCell ref="S19:T23"/>
-    <mergeCell ref="B29:C33"/>
-    <mergeCell ref="D29:H33"/>
-    <mergeCell ref="I29:M33"/>
-    <mergeCell ref="N29:R33"/>
-    <mergeCell ref="S29:T33"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
complete appCfgPage function ok base
</commit_message>
<xml_diff>
--- a/pb01_gui_develop_record.xlsx
+++ b/pb01_gui_develop_record.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{0D325905-AFF9-4647-B230-73E94501D303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D89B9BC5-6188-483B-B456-8585B1818C05}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{0D325905-AFF9-4647-B230-73E94501D303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E687F8C-D540-45CE-A973-DE8BE7108FD7}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="develop" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Index</t>
   </si>
@@ -1184,6 +1184,302 @@
         <charset val="134"/>
       </rPr>
       <t>中完成。</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">在开发 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PB01 GUI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">的项目中，出现偶尔 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">HID </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">返回空字符的现象，导致 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">GUI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>接收数据错误，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">debug </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">发现下位机工作没有问题，并且 用 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Bus Hound </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">观察，数据也正确返回给了 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">。
+</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>问题出在脚本调用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> hidapi </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">函数中。目前使用了两种方法，具体是什么原因，推测是 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">set_nonblocking(1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">导致。
+方法1：当出现数据返回错误后，关闭 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>hid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">，并重新打开。使用此方法，还是会出现数据返回错误，但在数据返回错误后，调用此方法，可以保证后续 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">hid </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>操作正确完成。
+方法2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">script </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">中打开 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">hid </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">后，不设置 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>blocking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。使用此方法后，目前没有再出现数据返回错误的现象。</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1294,11 +1590,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2029,6 +2325,138 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>56616</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>125506</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>564776</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>38618</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="图片 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC9D6C4E-34BE-4296-92D3-CEAD0D2982DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7882356" y="12508006"/>
+          <a:ext cx="2916080" cy="675112"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>44824</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>592998</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>71718</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="图片 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDA5A29D-65F7-4702-9577-7D006E89564A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4860664" y="15621001"/>
+          <a:ext cx="2956094" cy="833717"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>62198</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>89648</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>44824</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>73364</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="图片 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E426225F-9A58-4419-AEBA-B74F92B8511D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4878038" y="13996148"/>
+          <a:ext cx="1788566" cy="936216"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2348,13 +2776,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:T88"/>
+  <dimension ref="B2:T110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S59" sqref="S59:T73"/>
+      <selection pane="bottomRight" activeCell="U84" sqref="U84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2363,56 +2791,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4" t="s">
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="4"/>
+      <c r="T2" s="5"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
@@ -2897,7 +3325,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="3"/>
@@ -3929,14 +4357,20 @@
       <c r="T73" s="2"/>
     </row>
     <row r="74" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B74" s="2"/>
+      <c r="B74" s="2">
+        <v>10</v>
+      </c>
       <c r="C74" s="2"/>
-      <c r="D74" s="3"/>
+      <c r="D74" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
+      <c r="I74" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
@@ -3952,12 +4386,12 @@
     <row r="75" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
-      <c r="D75" s="3"/>
+      <c r="D75" s="6"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
+      <c r="I75" s="6"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
@@ -3973,12 +4407,12 @@
     <row r="76" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
-      <c r="D76" s="3"/>
+      <c r="D76" s="6"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
+      <c r="I76" s="6"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
@@ -3994,12 +4428,12 @@
     <row r="77" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
-      <c r="D77" s="3"/>
+      <c r="D77" s="6"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
-      <c r="I77" s="3"/>
+      <c r="I77" s="6"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
@@ -4015,12 +4449,12 @@
     <row r="78" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
-      <c r="D78" s="3"/>
+      <c r="D78" s="6"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
+      <c r="I78" s="6"/>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
@@ -4036,12 +4470,12 @@
     <row r="79" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
-      <c r="D79" s="3"/>
+      <c r="D79" s="6"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
-      <c r="I79" s="3"/>
+      <c r="I79" s="6"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
@@ -4057,12 +4491,12 @@
     <row r="80" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
-      <c r="D80" s="3"/>
+      <c r="D80" s="6"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
+      <c r="I80" s="6"/>
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
@@ -4078,12 +4512,12 @@
     <row r="81" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
-      <c r="D81" s="3"/>
+      <c r="D81" s="6"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
-      <c r="I81" s="3"/>
+      <c r="I81" s="6"/>
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
@@ -4243,73 +4677,540 @@
       <c r="S88" s="2"/>
       <c r="T88" s="2"/>
     </row>
+    <row r="89" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+      <c r="K89" s="3"/>
+      <c r="L89" s="3"/>
+      <c r="M89" s="3"/>
+      <c r="N89" s="3"/>
+      <c r="O89" s="3"/>
+      <c r="P89" s="3"/>
+      <c r="Q89" s="3"/>
+      <c r="R89" s="3"/>
+      <c r="S89" s="2"/>
+      <c r="T89" s="2"/>
+    </row>
+    <row r="90" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="3"/>
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+      <c r="P90" s="3"/>
+      <c r="Q90" s="3"/>
+      <c r="R90" s="3"/>
+      <c r="S90" s="2"/>
+      <c r="T90" s="2"/>
+    </row>
+    <row r="91" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
+      <c r="P91" s="3"/>
+      <c r="Q91" s="3"/>
+      <c r="R91" s="3"/>
+      <c r="S91" s="2"/>
+      <c r="T91" s="2"/>
+    </row>
+    <row r="92" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+      <c r="M92" s="3"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="3"/>
+      <c r="P92" s="3"/>
+      <c r="Q92" s="3"/>
+      <c r="R92" s="3"/>
+      <c r="S92" s="2"/>
+      <c r="T92" s="2"/>
+    </row>
+    <row r="93" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
+      <c r="I93" s="3"/>
+      <c r="J93" s="3"/>
+      <c r="K93" s="3"/>
+      <c r="L93" s="3"/>
+      <c r="M93" s="3"/>
+      <c r="N93" s="3"/>
+      <c r="O93" s="3"/>
+      <c r="P93" s="3"/>
+      <c r="Q93" s="3"/>
+      <c r="R93" s="3"/>
+      <c r="S93" s="2"/>
+      <c r="T93" s="2"/>
+    </row>
+    <row r="94" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
+      <c r="I94" s="3"/>
+      <c r="J94" s="3"/>
+      <c r="K94" s="3"/>
+      <c r="L94" s="3"/>
+      <c r="M94" s="3"/>
+      <c r="N94" s="3"/>
+      <c r="O94" s="3"/>
+      <c r="P94" s="3"/>
+      <c r="Q94" s="3"/>
+      <c r="R94" s="3"/>
+      <c r="S94" s="2"/>
+      <c r="T94" s="2"/>
+    </row>
+    <row r="95" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
+      <c r="I95" s="3"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="3"/>
+      <c r="L95" s="3"/>
+      <c r="M95" s="3"/>
+      <c r="N95" s="3"/>
+      <c r="O95" s="3"/>
+      <c r="P95" s="3"/>
+      <c r="Q95" s="3"/>
+      <c r="R95" s="3"/>
+      <c r="S95" s="2"/>
+      <c r="T95" s="2"/>
+    </row>
+    <row r="96" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
+      <c r="I96" s="3"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="3"/>
+      <c r="M96" s="3"/>
+      <c r="N96" s="3"/>
+      <c r="O96" s="3"/>
+      <c r="P96" s="3"/>
+      <c r="Q96" s="3"/>
+      <c r="R96" s="3"/>
+      <c r="S96" s="2"/>
+      <c r="T96" s="2"/>
+    </row>
+    <row r="97" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
+      <c r="I97" s="3"/>
+      <c r="J97" s="3"/>
+      <c r="K97" s="3"/>
+      <c r="L97" s="3"/>
+      <c r="M97" s="3"/>
+      <c r="N97" s="3"/>
+      <c r="O97" s="3"/>
+      <c r="P97" s="3"/>
+      <c r="Q97" s="3"/>
+      <c r="R97" s="3"/>
+      <c r="S97" s="2"/>
+      <c r="T97" s="2"/>
+    </row>
+    <row r="98" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="3"/>
+      <c r="I98" s="3"/>
+      <c r="J98" s="3"/>
+      <c r="K98" s="3"/>
+      <c r="L98" s="3"/>
+      <c r="M98" s="3"/>
+      <c r="N98" s="3"/>
+      <c r="O98" s="3"/>
+      <c r="P98" s="3"/>
+      <c r="Q98" s="3"/>
+      <c r="R98" s="3"/>
+      <c r="S98" s="2"/>
+      <c r="T98" s="2"/>
+    </row>
+    <row r="99" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3"/>
+      <c r="I99" s="3"/>
+      <c r="J99" s="3"/>
+      <c r="K99" s="3"/>
+      <c r="L99" s="3"/>
+      <c r="M99" s="3"/>
+      <c r="N99" s="3"/>
+      <c r="O99" s="3"/>
+      <c r="P99" s="3"/>
+      <c r="Q99" s="3"/>
+      <c r="R99" s="3"/>
+      <c r="S99" s="2"/>
+      <c r="T99" s="2"/>
+    </row>
+    <row r="100" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
+      <c r="H100" s="3"/>
+      <c r="I100" s="3"/>
+      <c r="J100" s="3"/>
+      <c r="K100" s="3"/>
+      <c r="L100" s="3"/>
+      <c r="M100" s="3"/>
+      <c r="N100" s="3"/>
+      <c r="O100" s="3"/>
+      <c r="P100" s="3"/>
+      <c r="Q100" s="3"/>
+      <c r="R100" s="3"/>
+      <c r="S100" s="2"/>
+      <c r="T100" s="2"/>
+    </row>
+    <row r="101" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+      <c r="I101" s="3"/>
+      <c r="J101" s="3"/>
+      <c r="K101" s="3"/>
+      <c r="L101" s="3"/>
+      <c r="M101" s="3"/>
+      <c r="N101" s="3"/>
+      <c r="O101" s="3"/>
+      <c r="P101" s="3"/>
+      <c r="Q101" s="3"/>
+      <c r="R101" s="3"/>
+      <c r="S101" s="2"/>
+      <c r="T101" s="2"/>
+    </row>
+    <row r="102" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
+      <c r="I102" s="3"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="3"/>
+      <c r="M102" s="3"/>
+      <c r="N102" s="3"/>
+      <c r="O102" s="3"/>
+      <c r="P102" s="3"/>
+      <c r="Q102" s="3"/>
+      <c r="R102" s="3"/>
+      <c r="S102" s="2"/>
+      <c r="T102" s="2"/>
+    </row>
+    <row r="103" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+      <c r="I103" s="3"/>
+      <c r="J103" s="3"/>
+      <c r="K103" s="3"/>
+      <c r="L103" s="3"/>
+      <c r="M103" s="3"/>
+      <c r="N103" s="3"/>
+      <c r="O103" s="3"/>
+      <c r="P103" s="3"/>
+      <c r="Q103" s="3"/>
+      <c r="R103" s="3"/>
+      <c r="S103" s="2"/>
+      <c r="T103" s="2"/>
+    </row>
+    <row r="104" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
+      <c r="I104" s="3"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
+      <c r="M104" s="3"/>
+      <c r="N104" s="3"/>
+      <c r="O104" s="3"/>
+      <c r="P104" s="3"/>
+      <c r="Q104" s="3"/>
+      <c r="R104" s="3"/>
+      <c r="S104" s="2"/>
+      <c r="T104" s="2"/>
+    </row>
+    <row r="105" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
+      <c r="I105" s="3"/>
+      <c r="J105" s="3"/>
+      <c r="K105" s="3"/>
+      <c r="L105" s="3"/>
+      <c r="M105" s="3"/>
+      <c r="N105" s="3"/>
+      <c r="O105" s="3"/>
+      <c r="P105" s="3"/>
+      <c r="Q105" s="3"/>
+      <c r="R105" s="3"/>
+      <c r="S105" s="2"/>
+      <c r="T105" s="2"/>
+    </row>
+    <row r="106" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
+      <c r="I106" s="3"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
+      <c r="M106" s="3"/>
+      <c r="N106" s="3"/>
+      <c r="O106" s="3"/>
+      <c r="P106" s="3"/>
+      <c r="Q106" s="3"/>
+      <c r="R106" s="3"/>
+      <c r="S106" s="2"/>
+      <c r="T106" s="2"/>
+    </row>
+    <row r="107" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="3"/>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
+      <c r="H107" s="3"/>
+      <c r="I107" s="3"/>
+      <c r="J107" s="3"/>
+      <c r="K107" s="3"/>
+      <c r="L107" s="3"/>
+      <c r="M107" s="3"/>
+      <c r="N107" s="3"/>
+      <c r="O107" s="3"/>
+      <c r="P107" s="3"/>
+      <c r="Q107" s="3"/>
+      <c r="R107" s="3"/>
+      <c r="S107" s="2"/>
+      <c r="T107" s="2"/>
+    </row>
+    <row r="108" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="3"/>
+      <c r="M108" s="3"/>
+      <c r="N108" s="3"/>
+      <c r="O108" s="3"/>
+      <c r="P108" s="3"/>
+      <c r="Q108" s="3"/>
+      <c r="R108" s="3"/>
+      <c r="S108" s="2"/>
+      <c r="T108" s="2"/>
+    </row>
+    <row r="109" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+      <c r="H109" s="3"/>
+      <c r="I109" s="3"/>
+      <c r="J109" s="3"/>
+      <c r="K109" s="3"/>
+      <c r="L109" s="3"/>
+      <c r="M109" s="3"/>
+      <c r="N109" s="3"/>
+      <c r="O109" s="3"/>
+      <c r="P109" s="3"/>
+      <c r="Q109" s="3"/>
+      <c r="R109" s="3"/>
+      <c r="S109" s="2"/>
+      <c r="T109" s="2"/>
+    </row>
+    <row r="110" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+      <c r="F110" s="3"/>
+      <c r="G110" s="3"/>
+      <c r="H110" s="3"/>
+      <c r="I110" s="3"/>
+      <c r="J110" s="3"/>
+      <c r="K110" s="3"/>
+      <c r="L110" s="3"/>
+      <c r="M110" s="3"/>
+      <c r="N110" s="3"/>
+      <c r="O110" s="3"/>
+      <c r="P110" s="3"/>
+      <c r="Q110" s="3"/>
+      <c r="R110" s="3"/>
+      <c r="S110" s="2"/>
+      <c r="T110" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="65">
+  <mergeCells count="70">
+    <mergeCell ref="B74:C95"/>
+    <mergeCell ref="D74:H95"/>
+    <mergeCell ref="I74:M95"/>
+    <mergeCell ref="N74:R95"/>
+    <mergeCell ref="S74:T95"/>
+    <mergeCell ref="B106:C110"/>
+    <mergeCell ref="D106:H110"/>
+    <mergeCell ref="I106:M110"/>
+    <mergeCell ref="N106:R110"/>
+    <mergeCell ref="S106:T110"/>
+    <mergeCell ref="B101:C105"/>
+    <mergeCell ref="D101:H105"/>
+    <mergeCell ref="I101:M105"/>
+    <mergeCell ref="N101:R105"/>
+    <mergeCell ref="S101:T105"/>
+    <mergeCell ref="B9:C15"/>
+    <mergeCell ref="D9:H15"/>
+    <mergeCell ref="I9:M15"/>
+    <mergeCell ref="N9:R15"/>
+    <mergeCell ref="S9:T15"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:H3"/>
+    <mergeCell ref="I2:M3"/>
+    <mergeCell ref="N2:R3"/>
+    <mergeCell ref="S2:T3"/>
+    <mergeCell ref="B21:C25"/>
+    <mergeCell ref="D21:H25"/>
+    <mergeCell ref="I21:M25"/>
+    <mergeCell ref="N21:R25"/>
+    <mergeCell ref="S21:T25"/>
+    <mergeCell ref="B16:C20"/>
+    <mergeCell ref="D16:H20"/>
+    <mergeCell ref="I16:M20"/>
+    <mergeCell ref="N16:R20"/>
+    <mergeCell ref="S16:T20"/>
+    <mergeCell ref="B26:C36"/>
+    <mergeCell ref="D26:H36"/>
+    <mergeCell ref="I26:M36"/>
+    <mergeCell ref="N26:R36"/>
+    <mergeCell ref="S26:T36"/>
+    <mergeCell ref="B37:C45"/>
+    <mergeCell ref="D37:H45"/>
+    <mergeCell ref="I37:M45"/>
+    <mergeCell ref="N37:R45"/>
+    <mergeCell ref="S37:T45"/>
+    <mergeCell ref="B46:C53"/>
+    <mergeCell ref="D46:H53"/>
+    <mergeCell ref="I46:M53"/>
+    <mergeCell ref="N46:R53"/>
+    <mergeCell ref="S46:T53"/>
+    <mergeCell ref="B54:C58"/>
+    <mergeCell ref="D54:H58"/>
+    <mergeCell ref="I54:M58"/>
+    <mergeCell ref="N54:R58"/>
+    <mergeCell ref="S54:T58"/>
+    <mergeCell ref="B59:C73"/>
+    <mergeCell ref="D59:H73"/>
+    <mergeCell ref="I59:M73"/>
+    <mergeCell ref="N59:R73"/>
+    <mergeCell ref="S59:T73"/>
+    <mergeCell ref="B96:C100"/>
+    <mergeCell ref="D96:H100"/>
+    <mergeCell ref="I96:M100"/>
+    <mergeCell ref="N96:R100"/>
+    <mergeCell ref="S96:T100"/>
     <mergeCell ref="B4:C8"/>
     <mergeCell ref="D4:H8"/>
     <mergeCell ref="I4:M8"/>
     <mergeCell ref="N4:R8"/>
     <mergeCell ref="S4:T8"/>
-    <mergeCell ref="B74:C78"/>
-    <mergeCell ref="D74:H78"/>
-    <mergeCell ref="I74:M78"/>
-    <mergeCell ref="N74:R78"/>
-    <mergeCell ref="S74:T78"/>
-    <mergeCell ref="B59:C73"/>
-    <mergeCell ref="D59:H73"/>
-    <mergeCell ref="I59:M73"/>
-    <mergeCell ref="N59:R73"/>
-    <mergeCell ref="S59:T73"/>
-    <mergeCell ref="B54:C58"/>
-    <mergeCell ref="D54:H58"/>
-    <mergeCell ref="I54:M58"/>
-    <mergeCell ref="N54:R58"/>
-    <mergeCell ref="S54:T58"/>
-    <mergeCell ref="B46:C53"/>
-    <mergeCell ref="D46:H53"/>
-    <mergeCell ref="I46:M53"/>
-    <mergeCell ref="N46:R53"/>
-    <mergeCell ref="S46:T53"/>
-    <mergeCell ref="B37:C45"/>
-    <mergeCell ref="D37:H45"/>
-    <mergeCell ref="I37:M45"/>
-    <mergeCell ref="N37:R45"/>
-    <mergeCell ref="S37:T45"/>
-    <mergeCell ref="B26:C36"/>
-    <mergeCell ref="D26:H36"/>
-    <mergeCell ref="I26:M36"/>
-    <mergeCell ref="N26:R36"/>
-    <mergeCell ref="S26:T36"/>
-    <mergeCell ref="B16:C20"/>
-    <mergeCell ref="D16:H20"/>
-    <mergeCell ref="I16:M20"/>
-    <mergeCell ref="N16:R20"/>
-    <mergeCell ref="S16:T20"/>
-    <mergeCell ref="B21:C25"/>
-    <mergeCell ref="D21:H25"/>
-    <mergeCell ref="I21:M25"/>
-    <mergeCell ref="N21:R25"/>
-    <mergeCell ref="S21:T25"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:H3"/>
-    <mergeCell ref="I2:M3"/>
-    <mergeCell ref="N2:R3"/>
-    <mergeCell ref="S2:T3"/>
-    <mergeCell ref="B9:C15"/>
-    <mergeCell ref="D9:H15"/>
-    <mergeCell ref="I9:M15"/>
-    <mergeCell ref="N9:R15"/>
-    <mergeCell ref="S9:T15"/>
-    <mergeCell ref="B79:C83"/>
-    <mergeCell ref="D79:H83"/>
-    <mergeCell ref="I79:M83"/>
-    <mergeCell ref="N79:R83"/>
-    <mergeCell ref="S79:T83"/>
-    <mergeCell ref="B84:C88"/>
-    <mergeCell ref="D84:H88"/>
-    <mergeCell ref="I84:M88"/>
-    <mergeCell ref="N84:R88"/>
-    <mergeCell ref="S84:T88"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4332,56 +5233,56 @@
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4" t="s">
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="4"/>
+      <c r="T2" s="5"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
@@ -5023,41 +5924,41 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B4:C8"/>
+    <mergeCell ref="D4:H8"/>
+    <mergeCell ref="I4:M8"/>
+    <mergeCell ref="N4:R8"/>
+    <mergeCell ref="S4:T8"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:H3"/>
+    <mergeCell ref="I2:M3"/>
+    <mergeCell ref="N2:R3"/>
+    <mergeCell ref="S2:T3"/>
+    <mergeCell ref="B14:C18"/>
+    <mergeCell ref="D14:H18"/>
+    <mergeCell ref="I14:M18"/>
+    <mergeCell ref="N14:R18"/>
+    <mergeCell ref="S14:T18"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="D9:H13"/>
+    <mergeCell ref="I9:M13"/>
+    <mergeCell ref="N9:R13"/>
+    <mergeCell ref="S9:T13"/>
+    <mergeCell ref="B24:C28"/>
+    <mergeCell ref="D24:H28"/>
+    <mergeCell ref="I24:M28"/>
+    <mergeCell ref="N24:R28"/>
+    <mergeCell ref="S24:T28"/>
+    <mergeCell ref="B19:C23"/>
+    <mergeCell ref="D19:H23"/>
+    <mergeCell ref="I19:M23"/>
+    <mergeCell ref="N19:R23"/>
+    <mergeCell ref="S19:T23"/>
     <mergeCell ref="B29:C33"/>
     <mergeCell ref="D29:H33"/>
     <mergeCell ref="I29:M33"/>
     <mergeCell ref="N29:R33"/>
     <mergeCell ref="S29:T33"/>
-    <mergeCell ref="B19:C23"/>
-    <mergeCell ref="D19:H23"/>
-    <mergeCell ref="I19:M23"/>
-    <mergeCell ref="N19:R23"/>
-    <mergeCell ref="S19:T23"/>
-    <mergeCell ref="B24:C28"/>
-    <mergeCell ref="D24:H28"/>
-    <mergeCell ref="I24:M28"/>
-    <mergeCell ref="N24:R28"/>
-    <mergeCell ref="S24:T28"/>
-    <mergeCell ref="B9:C13"/>
-    <mergeCell ref="D9:H13"/>
-    <mergeCell ref="I9:M13"/>
-    <mergeCell ref="N9:R13"/>
-    <mergeCell ref="S9:T13"/>
-    <mergeCell ref="B14:C18"/>
-    <mergeCell ref="D14:H18"/>
-    <mergeCell ref="I14:M18"/>
-    <mergeCell ref="N14:R18"/>
-    <mergeCell ref="S14:T18"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:H3"/>
-    <mergeCell ref="I2:M3"/>
-    <mergeCell ref="N2:R3"/>
-    <mergeCell ref="S2:T3"/>
-    <mergeCell ref="B4:C8"/>
-    <mergeCell ref="D4:H8"/>
-    <mergeCell ref="I4:M8"/>
-    <mergeCell ref="N4:R8"/>
-    <mergeCell ref="S4:T8"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>